<commit_message>
Adição de artigos e atualização de leituras.
</commit_message>
<xml_diff>
--- a/Scenario3/PesquisaScopus.xlsx
+++ b/Scenario3/PesquisaScopus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/MGTI/03 - Gestão Estratégica e do Conhecimento/Referencias_Aula5/WeakSignals/Scenario3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/Scenario3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587DF0A9-7049-2149-9E55-2A980BEB4B63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1803229-AC2C-534B-8EAC-AFE12A402232}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="24940" windowHeight="12680" activeTab="1" xr2:uid="{F0A6DCAD-C322-1B43-8143-01FC92096E1B}"/>
+    <workbookView xWindow="300" yWindow="460" windowWidth="24940" windowHeight="12680" xr2:uid="{F0A6DCAD-C322-1B43-8143-01FC92096E1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cenarios_Pesquisa_WeakSignals" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <r>
       <t>TITLE-ABS-KEY ( </t>
@@ -808,6 +808,179 @@
   </si>
   <si>
     <t>Chemistry</t>
+  </si>
+  <si>
+    <t>pesquisa5</t>
+  </si>
+  <si>
+    <r>
+      <t>( TITLE-ABS-KEY ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"weak signals"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) )  AND  ( ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"big data"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"corporate"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"foresight"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) OR  ( "wild cards" ) )  AND  ( LIMIT-TO ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"BUSI"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  LIMIT-TO ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"SOCI"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  LIMIT-TO ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"COMP"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  LIMIT-TO ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"ECON"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  LIMIT-TO ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"DECI"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) )</t>
+    </r>
+  </si>
+  <si>
+    <t>Feita após encontrar alguns artigos interessantes sobre o assunto e ver que ele está diretamente relacionado com o trabalho.</t>
   </si>
 </sst>
 </file>
@@ -877,9 +1050,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -891,6 +1061,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF0166F-787D-894D-8190-7C9C1739C3CD}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,7 +1414,7 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="10">
         <f>C3+C4+C5+C6+C7</f>
         <v>298</v>
       </c>
@@ -1253,7 +1426,7 @@
       <c r="C4">
         <v>30</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" ht="23" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1262,7 +1435,7 @@
       <c r="C5">
         <v>21</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" ht="23" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1271,7 +1444,7 @@
       <c r="C6">
         <v>126</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" ht="23" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -1280,7 +1453,7 @@
       <c r="C7">
         <v>114</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1304,14 +1477,14 @@
         <v>3407</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>201</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1328,8 +1501,19 @@
       <c r="C11">
         <v>178</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="144" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1344,7 +1528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BBB1CB-C67A-0243-BD1D-82E368B732D1}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1354,31 +1538,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="9">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B4">
@@ -1386,23 +1570,23 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B7">
@@ -1410,7 +1594,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B8">
@@ -1418,7 +1602,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B9">
@@ -1426,7 +1610,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B10">
@@ -1434,7 +1618,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B11">
@@ -1442,7 +1626,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B12">
@@ -1450,7 +1634,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B13">
@@ -1458,7 +1642,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B14">
@@ -1466,7 +1650,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B15">
@@ -1474,7 +1658,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B16">
@@ -1482,7 +1666,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B17">
@@ -1490,7 +1674,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B18">

</xml_diff>

<commit_message>
Muitas coisas feitas... nova pesquisa, novos artigos sugeridos pela prof Elaine, novas leituras finalizadas... dentre outras coisas.
</commit_message>
<xml_diff>
--- a/Scenario3/PesquisaScopus.xlsx
+++ b/Scenario3/PesquisaScopus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/Scenario3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D954BC4-E808-D648-8BD2-560666028FFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EA93BC-4A09-5A4D-BEB6-3D84A8D5769A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="-20580" windowWidth="33240" windowHeight="19300" xr2:uid="{F0A6DCAD-C322-1B43-8143-01FC92096E1B}"/>
+    <workbookView xWindow="80" yWindow="-20580" windowWidth="33240" windowHeight="19300" xr2:uid="{F0A6DCAD-C322-1B43-8143-01FC92096E1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cenarios_Pesquisa_WeakSignals" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <r>
       <t>TITLE-ABS-KEY ( </t>
@@ -982,6 +982,626 @@
   </si>
   <si>
     <t>Feita após encontrar alguns artigos interessantes sobre o assunto e ver que ele está diretamente relacionado com o trabalho.</t>
+  </si>
+  <si>
+    <t>pesquisa6</t>
+  </si>
+  <si>
+    <r>
+      <t>( TITLE-ABS-KEY ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"weak signals"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) )  AND  ( ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"scenario"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"planning"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"big"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"data"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"scanning"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"corporate"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"foresight"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"wild cards"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"future"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"horizon scanning"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"text mining"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"inovation"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"enviromental"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"early warnings"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"prospective"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) )  AND  ( EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"ENGI"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"PHYS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"BIOC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"MEDI"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"EART"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"CHEM"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"AGRI"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"NEUR"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"PSYC"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"ENER"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"ARTS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"IMMU"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"PHAR"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"CENG"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"HEAL"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"VETE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  OR  EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"DENT"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) )  AND  ( EXCLUDE ( SUBJAREA ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Undefined"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) ) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1379,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF0166F-787D-894D-8190-7C9C1739C3CD}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1518,6 +2138,14 @@
       </c>
       <c r="D12" s="4" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="408" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusão de uma nova pesquisa feita e início dos trabalhos dos artigos dentro dessa pesquisa
</commit_message>
<xml_diff>
--- a/Scenario3/PesquisaScopus.xlsx
+++ b/Scenario3/PesquisaScopus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\weak_signals\Scenario3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DB06A8-859B-4DCD-B233-5788F81FDE68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E013BFE0-2FB2-4595-BDD1-70E513F30B1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F0A6DCAD-C322-1B43-8143-01FC92096E1B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <r>
       <t>TITLE-ABS-KEY ( </t>
@@ -1919,6 +1919,101 @@
   </si>
   <si>
     <t>( TITLE-ABS-KEY ( "foresight" ) )  AND  PUBYEAR  &gt;  2009 and "weak signals" or "scenario" or "planning" or "big" or "data" or "big data" or "horizon" or  "scanning" or "horizon scanning" or "corporate" or "wild cards" or "future" or "text mining" or "innovation" or "environmental" or "early warnings" or "prospective" or "forecasting" or "strategic"</t>
+  </si>
+  <si>
+    <r>
+      <t>( ( ( TITLE-ABS-KEY ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"foresight"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> )  AND  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"competitive intelligence"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>  OR  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"big data"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>  OR  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"forecast"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) )  AND  PUBYEAR  &gt;  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2009</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF969696"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> ) ) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1986,7 +2081,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2007,10 +2102,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2325,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF0166F-787D-894D-8190-7C9C1739C3CD}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2362,7 +2460,7 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="12">
         <f>C3+C4+C5+C6+C7</f>
         <v>298</v>
       </c>
@@ -2374,7 +2472,7 @@
       <c r="C4">
         <v>30</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
@@ -2383,7 +2481,7 @@
       <c r="C5">
         <v>21</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="12"/>
     </row>
     <row r="6" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
@@ -2392,7 +2490,7 @@
       <c r="C6">
         <v>126</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
@@ -2401,7 +2499,7 @@
       <c r="C7">
         <v>114</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -2487,7 +2585,15 @@
       <c r="B15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" ht="69.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
+        <v>708</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>